<commit_message>
5 + 7 + 8
</commit_message>
<xml_diff>
--- a/Лабораторные работы/№ 5/№ 5.xlsx
+++ b/Лабораторные работы/№ 5/№ 5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Разработки разработчика\Lesson_repo\Лабораторные работы\№ 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47763420-12A7-46D9-9FDA-54D298EE5EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5F4BB5-903C-4862-BB5C-10AF120C1C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,6 +30,7 @@
   <definedNames>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'Задание 1'!$B$13:$E$15</definedName>
     <definedName name="solver_adj" localSheetId="11" hidden="1">'Задача 10'!$G$2:$G$3</definedName>
+    <definedName name="solver_adj" localSheetId="12" hidden="1">'Задача 11'!$B$15:$B$19</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'Задача 2'!$B$13:$D$15</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'Задача 3'!$B$12:$E$13</definedName>
     <definedName name="solver_adj" localSheetId="5" hidden="1">'Задача 4'!$B$12:$E$14</definedName>
@@ -41,6 +42,7 @@
     <definedName name="solver_adj" localSheetId="0" hidden="1">Лист1!$B$13:$F$16</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="11" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="12" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
@@ -52,6 +54,7 @@
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
@@ -64,6 +67,7 @@
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
@@ -75,6 +79,7 @@
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
@@ -86,6 +91,7 @@
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="12" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
@@ -97,6 +103,7 @@
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Задание 1'!$B$13:$E$15</definedName>
     <definedName name="solver_lhs1" localSheetId="11" hidden="1">'Задача 10'!$E$7</definedName>
+    <definedName name="solver_lhs1" localSheetId="12" hidden="1">'Задача 11'!$E$16</definedName>
     <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Задача 2'!$B$13:$D$15</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">'Задача 3'!$B$12:$E$13</definedName>
     <definedName name="solver_lhs1" localSheetId="5" hidden="1">'Задача 4'!$B$12:$E$14</definedName>
@@ -108,6 +115,7 @@
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Лист1!$B$13:$F$16</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Задание 1'!$B$16:$E$16</definedName>
     <definedName name="solver_lhs2" localSheetId="11" hidden="1">'Задача 10'!$E$8</definedName>
+    <definedName name="solver_lhs2" localSheetId="12" hidden="1">'Задача 11'!$E$17</definedName>
     <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Задача 2'!$B$16:$D$16</definedName>
     <definedName name="solver_lhs2" localSheetId="4" hidden="1">'Задача 3'!$B$14:$E$14</definedName>
     <definedName name="solver_lhs2" localSheetId="5" hidden="1">'Задача 4'!$B$15:$E$15</definedName>
@@ -119,6 +127,7 @@
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Лист1!$B$17:$F$17</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Задание 1'!$F$13:$F$15</definedName>
     <definedName name="solver_lhs3" localSheetId="11" hidden="1">'Задача 10'!$G$2</definedName>
+    <definedName name="solver_lhs3" localSheetId="12" hidden="1">'Задача 11'!$E$18</definedName>
     <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Задача 2'!$E$13:$E$15</definedName>
     <definedName name="solver_lhs3" localSheetId="4" hidden="1">'Задача 3'!$F$12:$F$13</definedName>
     <definedName name="solver_lhs3" localSheetId="5" hidden="1">'Задача 4'!$F$12:$F$14</definedName>
@@ -127,10 +136,12 @@
     <definedName name="solver_lhs3" localSheetId="10" hidden="1">'Задача 9'!$F$12</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Лист1!$G$13:$G$16</definedName>
     <definedName name="solver_lhs4" localSheetId="11" hidden="1">'Задача 10'!$G$3</definedName>
+    <definedName name="solver_lhs4" localSheetId="12" hidden="1">'Задача 11'!$E$19</definedName>
     <definedName name="solver_lhs4" localSheetId="6" hidden="1">'Задача 5'!$F$16</definedName>
     <definedName name="solver_lhs4" localSheetId="7" hidden="1">'Задача 6'!$F$9</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="12" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
@@ -142,6 +153,7 @@
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="11" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="12" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
@@ -153,6 +165,7 @@
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="11" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="12" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
@@ -164,6 +177,7 @@
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="12" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
@@ -176,6 +190,7 @@
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
@@ -187,6 +202,7 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="12" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
@@ -199,6 +215,7 @@
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="11" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="12" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="5" hidden="1">3</definedName>
@@ -210,6 +227,7 @@
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
@@ -222,6 +240,7 @@
     <definedName name="solver_opt" localSheetId="1" hidden="1">'Задание 0 - не то'!$B$22</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'Задание 1'!$B$19</definedName>
     <definedName name="solver_opt" localSheetId="11" hidden="1">'Задача 10'!$B$11</definedName>
+    <definedName name="solver_opt" localSheetId="12" hidden="1">'Задача 11'!$E$15</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">'Задача 2'!$B$19</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">'Задача 3'!$B$17</definedName>
     <definedName name="solver_opt" localSheetId="5" hidden="1">'Задача 4'!$B$18</definedName>
@@ -233,6 +252,7 @@
     <definedName name="solver_opt" localSheetId="0" hidden="1">Лист1!$B$20</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="11" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="12" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
@@ -244,6 +264,7 @@
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
@@ -255,6 +276,7 @@
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="12" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="5" hidden="1">3</definedName>
@@ -266,6 +288,7 @@
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="12" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="5" hidden="1">2</definedName>
@@ -277,6 +300,7 @@
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="12" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="5" hidden="1">2</definedName>
@@ -285,10 +309,12 @@
     <definedName name="solver_rel3" localSheetId="10" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel4" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="12" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="7" hidden="1">2</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="11" hidden="1">'Задача 10'!$D$3</definedName>
+    <definedName name="solver_rhs1" localSheetId="12" hidden="1">'Задача 11'!$B$9</definedName>
     <definedName name="solver_rhs1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="5" hidden="1">0</definedName>
@@ -300,6 +326,7 @@
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">'Задание 1'!$B$17:$E$17</definedName>
     <definedName name="solver_rhs2" localSheetId="11" hidden="1">'Задача 10'!$D$4</definedName>
+    <definedName name="solver_rhs2" localSheetId="12" hidden="1">'Задача 11'!$B$10</definedName>
     <definedName name="solver_rhs2" localSheetId="3" hidden="1">'Задача 2'!$B$17:$D$17</definedName>
     <definedName name="solver_rhs2" localSheetId="4" hidden="1">'Задача 3'!$B$15:$E$15</definedName>
     <definedName name="solver_rhs2" localSheetId="5" hidden="1">'Задача 4'!$B$16:$E$16</definedName>
@@ -311,6 +338,7 @@
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Лист1!$B$18:$F$18</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">'Задание 1'!$G$13:$G$15</definedName>
     <definedName name="solver_rhs3" localSheetId="11" hidden="1">3</definedName>
+    <definedName name="solver_rhs3" localSheetId="12" hidden="1">'Задача 11'!$B$11</definedName>
     <definedName name="solver_rhs3" localSheetId="3" hidden="1">'Задача 2'!$F$13:$F$15</definedName>
     <definedName name="solver_rhs3" localSheetId="4" hidden="1">'Задача 3'!$G$12:$G$13</definedName>
     <definedName name="solver_rhs3" localSheetId="5" hidden="1">'Задача 4'!$G$12:$G$14</definedName>
@@ -319,10 +347,12 @@
     <definedName name="solver_rhs3" localSheetId="10" hidden="1">'Задача 9'!$B$8</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">Лист1!$H$13:$H$16</definedName>
     <definedName name="solver_rhs4" localSheetId="11" hidden="1">'Задача 10'!$G$4</definedName>
+    <definedName name="solver_rhs4" localSheetId="12" hidden="1">'Задача 11'!$B$12</definedName>
     <definedName name="solver_rhs4" localSheetId="6" hidden="1">'Задача 5'!$F$5</definedName>
     <definedName name="solver_rhs4" localSheetId="7" hidden="1">'Задача 6'!$H$9</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="12" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
@@ -334,6 +364,7 @@
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="12" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
@@ -345,6 +376,7 @@
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="12" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
@@ -356,6 +388,7 @@
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="12" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
@@ -367,6 +400,7 @@
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="11" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="12" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
@@ -378,6 +412,7 @@
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="11" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="12" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
@@ -389,6 +424,7 @@
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="11" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="12" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
@@ -401,6 +437,7 @@
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="11" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="12" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="5" hidden="1">2</definedName>
@@ -413,6 +450,7 @@
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="11" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="12" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
@@ -425,6 +463,7 @@
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="11" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="12" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
@@ -454,7 +493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="96">
   <si>
     <t>Стоимость перевозок</t>
   </si>
@@ -736,6 +775,12 @@
   </si>
   <si>
     <t>Минимальные ограничения диеты</t>
+  </si>
+  <si>
+    <t>Суш. рыба</t>
+  </si>
+  <si>
+    <t>Общие параметры</t>
   </si>
 </sst>
 </file>
@@ -1879,12 +1924,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1892,15 +1937,20 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7ABF7D-5290-41C5-A0D4-A1658440DDEB}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>85</v>
       </c>
@@ -1914,13 +1964,10 @@
         <v>88</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1940,7 +1987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -1960,7 +2007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1980,7 +2027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -2000,7 +2047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2020,7 +2067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>93</v>
       </c>
@@ -2028,7 +2075,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -2036,7 +2083,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -2044,7 +2091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -2052,7 +2099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -2060,9 +2107,96 @@
         <v>40</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <f>B15*B6+B16*C6+B17*D6+B18*E6+B19*F6</f>
+        <v>150.00000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16">
+        <f>B15*B2+B16*C2+B17*D2+B18*E2+B19*F2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17">
+        <v>0.83333333333333315</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17">
+        <f>B15*B3+B16*C3+B17*D3+B18*E3+B19*F3</f>
+        <v>30.000000000000011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18">
+        <v>5.0000000000000027</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18">
+        <f>B15*B4+B16*C4+B17*D4+B18*E4+B19*F4</f>
+        <v>15.833333333333332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19">
+        <v>3.333333333333333</v>
+      </c>
+      <c r="D19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19">
+        <f>B15*B5+B16*C5+B17*D5+B18*E5+B19*F5</f>
+        <v>40.000000000000014</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2406,7 +2540,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>